<commit_message>
Support and idp modification
</commit_message>
<xml_diff>
--- a/data/SupportData_2.xlsx
+++ b/data/SupportData_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashrafmahmoud/Documents/ITI/9 Months/Core courses/Data Visualization/Project/Story-of-Palestine-Dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E357E54-CBC1-0D45-AE7B-6581C113AAC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F303E2-51C7-0E4A-8956-4B9A40E61846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{BFF75450-91FB-1048-9915-987CF1EDE763}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{BFF75450-91FB-1048-9915-987CF1EDE763}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>Call For a Ceasefire</t>
   </si>
   <si>
-    <t>Call and Email your representative in the congress and demand a ceasefire. Lives can be saved in Gaza just by putting enough pressure on Politicians that in turn put pressure on Israel to stop this massacre.</t>
-  </si>
-  <si>
     <t>https://act.uscpr.org/a/callforgaza</t>
   </si>
   <si>
@@ -65,12 +62,6 @@
     <t>Spread The Word</t>
   </si>
   <si>
-    <t>Amplify the voices of those shining a light on the human rights abuses being committed by the IDF against the people of Gaza; otherwise, no one will know anything to stop them. Don't hesitate to share this website and engage in debates to make clear of the truth.</t>
-  </si>
-  <si>
-    <t>https://twitter.com/intent/tweet?url=${link}&amp;text=${text}</t>
-  </si>
-  <si>
     <t>hamas.jpeg</t>
   </si>
   <si>
@@ -108,6 +99,15 @@
   </si>
   <si>
     <t>link</t>
+  </si>
+  <si>
+    <t>Amplify the voices of those shining a light on the human rights abuses being committed by the IDF against the people of Gaza; otherwise, no one will know anything to stop them. Don't hesitate to share the truth.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call and Email your representative in the congress and demand a ceasefire. Lives can be saved in Gaza just by putting enough pressure on Politicians that in turn put pressure on Israel to stop this massacre.                                                                   </t>
+  </si>
+  <si>
+    <t>https://twitter.com/intent/tweet?url=Learn more about the story of Palestine, the status of Gaza, Israeli war crimes. Support Palestine!, https://story-of-palestine-dashboard.onrender.com/</t>
   </si>
 </sst>
 </file>
@@ -152,7 +152,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -160,6 +160,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -495,32 +497,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD6B8648-B7CF-134A-B714-0E74102A5FB1}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="213.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="139.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="155.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -528,78 +530,87 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>19</v>
-      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C10" s="3"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C17" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{7D42EA62-561B-164D-A411-E1906C41D1B2}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{E7FC0621-19C5-804E-A284-4A2A55A27D1C}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{46EDA75A-8904-FE44-B9B3-D8FC1B6AD1CE}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{7EC9B1A6-D547-2746-9114-319A11C52AFB}"/>
-    <hyperlink ref="C6" r:id="rId5" location=":~:text=O%20Allah%2C%20help%20and%20protect,in%20this%20time%20of%20crisis." xr:uid="{86EDADEE-E689-9C4A-AF2A-63BEA423C794}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{7EC9B1A6-D547-2746-9114-319A11C52AFB}"/>
+    <hyperlink ref="C6" r:id="rId4" location=":~:text=O%20Allah%2C%20help%20and%20protect,in%20this%20time%20of%20crisis." xr:uid="{86EDADEE-E689-9C4A-AF2A-63BEA423C794}"/>
+    <hyperlink ref="C4" r:id="rId5" display="https://twitter.com/intent/tweet?url=Learn more about the story of Palestine, the status of Gaza, Israeli war crimes. Support Palestine!, " xr:uid="{46EDA75A-8904-FE44-B9B3-D8FC1B6AD1CE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>